<commit_message>
update refresh, teams, reset list
</commit_message>
<xml_diff>
--- a/output_data/1.5-2.0.xlsx
+++ b/output_data/1.5-2.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Desktop\SoccerPro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Desktop\SoccerPro\soccerpro\output_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD6CDFC-49C0-4E11-A845-67A96E86D885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472569C7-ED9A-46AD-A983-0144C870943E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="234">
   <si>
     <t>index</t>
   </si>
@@ -82,6 +82,9 @@
     <t>Hypothesis</t>
   </si>
   <si>
+    <t>Scores</t>
+  </si>
+  <si>
     <t>https://www.flashscore.com.ng/match/GtnFNGnI/#/match-summary</t>
   </si>
   <si>
@@ -124,6 +127,9 @@
     <t>('Ebbsfleet', '2TIW')</t>
   </si>
   <si>
+    <t>1 - 4</t>
+  </si>
+  <si>
     <t>https://www.flashscore.com.ng/match/A7wjPTNM/#/match-summary</t>
   </si>
   <si>
@@ -199,6 +205,9 @@
     <t>('Welling', '2TIH')</t>
   </si>
   <si>
+    <t>0 - 4</t>
+  </si>
+  <si>
     <t>https://www.flashscore.com.ng/match/8Gr7PxI5/#/match-summary</t>
   </si>
   <si>
@@ -229,6 +238,9 @@
     <t>('Southend', '2TIW')</t>
   </si>
   <si>
+    <t>1 - 1</t>
+  </si>
+  <si>
     <t>https://www.flashscore.com.ng/match/6ksAJWkh/#/match-summary</t>
   </si>
   <si>
@@ -262,6 +274,9 @@
     <t>('Scotland', '2TIH')</t>
   </si>
   <si>
+    <t>1 - 3</t>
+  </si>
+  <si>
     <t>https://www.flashscore.com.ng/match/IJcgrWU3/#/match-summary</t>
   </si>
   <si>
@@ -289,12 +304,12 @@
     <t>['Cyprus', 'Kosovo']</t>
   </si>
   <si>
-    <t>0 - 4</t>
-  </si>
-  <si>
     <t>('Cyprus', '2TIW')</t>
   </si>
   <si>
+    <t>1 - 2</t>
+  </si>
+  <si>
     <t>https://www.flashscore.com.ng/match/ryUZshGJ/#/match-summary</t>
   </si>
   <si>
@@ -325,6 +340,9 @@
     <t>('Bulgaria', '2TIW')</t>
   </si>
   <si>
+    <t>0 - 0</t>
+  </si>
+  <si>
     <t>https://www.flashscore.com.ng/match/6gZd9X9f/#/match-summary</t>
   </si>
   <si>
@@ -349,6 +367,9 @@
     <t>('Lithuania', '2TIH')</t>
   </si>
   <si>
+    <t>0 - 3</t>
+  </si>
+  <si>
     <t>https://www.flashscore.com.ng/match/MRjKMvLF/#/match-summary</t>
   </si>
   <si>
@@ -376,9 +397,6 @@
     <t>['Triestina', 'Pro Vercelli']</t>
   </si>
   <si>
-    <t>1 - 1</t>
-  </si>
-  <si>
     <t>('Pro Vercelli', '2TIH')</t>
   </si>
   <si>
@@ -406,9 +424,6 @@
     <t>('Atalanta U23', '1TIW')</t>
   </si>
   <si>
-    <t>1 - 3</t>
-  </si>
-  <si>
     <t>['Padova', 'L.R. Vicenza']</t>
   </si>
   <si>
@@ -448,6 +463,9 @@
     <t>('Barendrecht', '2TIH')</t>
   </si>
   <si>
+    <t>2 - 5</t>
+  </si>
+  <si>
     <t>https://www.flashscore.com.ng/match/MJdPh2pT/#/match-summary</t>
   </si>
   <si>
@@ -478,6 +496,9 @@
     <t>('Antigua and Barbuda', '2TIW')</t>
   </si>
   <si>
+    <t>1 - 6</t>
+  </si>
+  <si>
     <t>https://www.flashscore.com.ng/match/GQk1omB6/#/match-summary</t>
   </si>
   <si>
@@ -502,6 +523,9 @@
     <t>('Glentoran', '2TIH')</t>
   </si>
   <si>
+    <t>2 - 3</t>
+  </si>
+  <si>
     <t>https://www.flashscore.com.ng/match/CztUWOcK/#/match-summary</t>
   </si>
   <si>
@@ -529,6 +553,9 @@
     <t>('Institute', '2TIH')</t>
   </si>
   <si>
+    <t>4 - 0</t>
+  </si>
+  <si>
     <t>https://www.flashscore.com.ng/match/UHeq9siU/#/match-summary</t>
   </si>
   <si>
@@ -577,9 +604,6 @@
     <t>('Afan Lido', '1TIW')</t>
   </si>
   <si>
-    <t>0 - 3</t>
-  </si>
-  <si>
     <t>['Cambrian United', 'Ammanford']</t>
   </si>
   <si>
@@ -692,9 +716,6 @@
   </si>
   <si>
     <t>('Aarau', '1TIW')</t>
-  </si>
-  <si>
-    <t>0 - 0</t>
   </si>
   <si>
     <t>['Schalke', 'Hertha Berlin']</t>
@@ -707,7 +728,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -719,6 +740,26 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -753,16 +794,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1063,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1074,7 +1120,7 @@
     <col min="4" max="4" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1135,240 +1181,255 @@
       <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="V1" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O2" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="V2" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="M3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="O3" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="V3" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="M4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O4" t="s">
-        <v>58</v>
+        <v>60</v>
+      </c>
+      <c r="V4" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" t="s">
         <v>59</v>
       </c>
-      <c r="C5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" t="s">
-        <v>65</v>
-      </c>
-      <c r="I5" t="s">
-        <v>66</v>
-      </c>
-      <c r="J5" t="s">
-        <v>57</v>
-      </c>
       <c r="K5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O5" t="s">
-        <v>68</v>
+        <v>71</v>
+      </c>
+      <c r="V5" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="M6" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="N6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="P6">
         <v>3</v>
@@ -1385,52 +1446,55 @@
       <c r="T6" t="b">
         <v>0</v>
       </c>
+      <c r="V6" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E7" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F7" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="G7" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="H7" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="I7" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="J7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L7" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="M7" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="N7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O7" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="P7">
         <v>6</v>
@@ -1447,52 +1511,55 @@
       <c r="T7" t="b">
         <v>0</v>
       </c>
+      <c r="V7" t="s">
+        <v>95</v>
+      </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D8" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E8" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="F8" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H8" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="I8" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="J8" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="K8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L8" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="M8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="O8" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="P8">
         <v>1</v>
@@ -1509,52 +1576,55 @@
       <c r="T8" t="b">
         <v>0</v>
       </c>
+      <c r="V8" t="s">
+        <v>106</v>
+      </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D9" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="E9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F9" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="G9" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="H9" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="I9" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="J9" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="K9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L9" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="M9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O9" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="P9">
         <v>3</v>
@@ -1571,52 +1641,55 @@
       <c r="T9" t="b">
         <v>0</v>
       </c>
+      <c r="V9" t="s">
+        <v>115</v>
+      </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="D10" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E10" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="F10" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="G10" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="H10" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="I10" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="J10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L10" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="M10" t="s">
-        <v>118</v>
+        <v>72</v>
       </c>
       <c r="N10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O10" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="P10">
         <v>5</v>
@@ -1633,52 +1706,55 @@
       <c r="T10" t="b">
         <v>0</v>
       </c>
+      <c r="V10" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C11" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D11" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="E11" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="F11" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="G11" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="H11" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="I11" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="J11" t="s">
-        <v>128</v>
+        <v>84</v>
       </c>
       <c r="K11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L11" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O11" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="P11">
         <v>12</v>
@@ -1695,52 +1771,55 @@
       <c r="T11" t="b">
         <v>0</v>
       </c>
+      <c r="V11" t="s">
+        <v>103</v>
+      </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C12" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D12" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="E12" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="F12" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G12" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H12" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="I12" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J12" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="K12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L12" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="M12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O12" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="P12">
         <v>13</v>
@@ -1757,52 +1836,55 @@
       <c r="T12" t="b">
         <v>0</v>
       </c>
+      <c r="V12" t="s">
+        <v>147</v>
+      </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D13" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E13" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="F13" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="G13" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H13" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="I13" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="J13" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="K13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L13" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="M13" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="N13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O13" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="P13">
         <v>3</v>
@@ -1819,52 +1901,55 @@
       <c r="T13" t="b">
         <v>0</v>
       </c>
+      <c r="V13" t="s">
+        <v>158</v>
+      </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>152</v>
+      <c r="B14" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="C14" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D14" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E14" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="F14" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14" t="s">
+        <v>162</v>
+      </c>
+      <c r="H14" t="s">
+        <v>163</v>
+      </c>
+      <c r="I14" t="s">
+        <v>164</v>
+      </c>
+      <c r="J14" t="s">
+        <v>82</v>
+      </c>
+      <c r="K14" t="s">
+        <v>30</v>
+      </c>
+      <c r="L14" t="s">
+        <v>165</v>
+      </c>
+      <c r="M14" t="s">
         <v>84</v>
       </c>
-      <c r="G14" t="s">
-        <v>155</v>
-      </c>
-      <c r="H14" t="s">
-        <v>156</v>
-      </c>
-      <c r="I14" t="s">
-        <v>157</v>
-      </c>
-      <c r="J14" t="s">
-        <v>78</v>
-      </c>
-      <c r="K14" t="s">
-        <v>29</v>
-      </c>
-      <c r="L14" t="s">
-        <v>158</v>
-      </c>
-      <c r="M14" t="s">
-        <v>128</v>
-      </c>
       <c r="N14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="O14" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="P14">
         <v>5</v>
@@ -1878,55 +1963,58 @@
       <c r="S14">
         <v>4</v>
       </c>
-      <c r="T14" t="b">
+      <c r="T14" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="V14" t="s">
+        <v>167</v>
+      </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="C15" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="D15" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="E15" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="F15" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="G15" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="H15" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="I15" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="J15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L15" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="M15" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O15" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="P15">
         <v>8</v>
@@ -1943,52 +2031,55 @@
       <c r="T15" t="b">
         <v>0</v>
       </c>
+      <c r="V15" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="C16" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="D16" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="E16" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="F16" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="G16" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="H16" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="I16" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="J16" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="K16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L16" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="M16" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N16" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="O16" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="P16">
         <v>10</v>
@@ -2002,55 +2093,58 @@
       <c r="S16">
         <v>2</v>
       </c>
-      <c r="T16" t="b">
+      <c r="T16" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="V16" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="C17" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="D17" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="E17" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="F17" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="G17" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="H17" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="I17" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="J17" t="s">
-        <v>185</v>
+        <v>115</v>
       </c>
       <c r="K17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L17" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="M17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O17" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="P17">
         <v>12</v>
@@ -2067,52 +2161,55 @@
       <c r="T17" t="b">
         <v>0</v>
       </c>
+      <c r="V17" t="s">
+        <v>144</v>
+      </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C18" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="D18" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="E18" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="F18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G18" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="H18" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="I18" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="J18" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="K18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L18" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="M18" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="N18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O18" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="P18">
         <v>8</v>
@@ -2129,52 +2226,55 @@
       <c r="T18" t="b">
         <v>0</v>
       </c>
+      <c r="V18" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="C19" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="D19" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="E19" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="F19" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="G19" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="H19" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="I19" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="J19" t="s">
-        <v>118</v>
+        <v>72</v>
       </c>
       <c r="K19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L19" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="M19" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="N19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O19" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="P19">
         <v>4</v>
@@ -2191,52 +2291,55 @@
       <c r="T19" t="b">
         <v>0</v>
       </c>
+      <c r="V19" t="s">
+        <v>115</v>
+      </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="C20" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="D20" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="E20" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="F20" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G20" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="H20" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="I20" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="J20" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="K20" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L20" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="M20" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="N20" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="O20" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="P20">
         <v>16</v>
@@ -2250,55 +2353,58 @@
       <c r="S20">
         <v>2</v>
       </c>
-      <c r="T20" t="b">
+      <c r="T20" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="V20" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="C21" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="D21" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="E21" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="F21" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="G21" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="H21" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="I21" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="J21" t="s">
-        <v>224</v>
+        <v>106</v>
       </c>
       <c r="K21" t="s">
+        <v>33</v>
+      </c>
+      <c r="L21" t="s">
+        <v>232</v>
+      </c>
+      <c r="M21" t="s">
         <v>32</v>
       </c>
-      <c r="L21" t="s">
-        <v>225</v>
-      </c>
-      <c r="M21" t="s">
-        <v>31</v>
-      </c>
       <c r="N21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O21" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="P21">
         <v>16</v>
@@ -2312,11 +2418,17 @@
       <c r="S21">
         <v>2</v>
       </c>
-      <c r="T21" t="b">
+      <c r="T21" s="3" t="b">
         <v>1</v>
+      </c>
+      <c r="V21" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B14" r:id="rId1" location="/match-summary" xr:uid="{5C3520AA-A280-4880-8521-FA874DD5FA9B}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>